<commit_message>
Make changes after draft revision feedback
</commit_message>
<xml_diff>
--- a/data/processed/classification-expset-1/powercalcs.xlsx
+++ b/data/processed/classification-expset-1/powercalcs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t>Mote</t>
   </si>
@@ -239,6 +239,14 @@
   </si>
   <si>
     <t>Low-Power C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1289,117 +1297,127 @@
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>22</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="8">
         <v>34</v>
       </c>
-      <c r="F43" s="6">
+      <c r="D43">
+        <v>52</v>
+      </c>
+      <c r="E43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="9">
         <f>1/5</f>
         <v>0.2</v>
       </c>
-      <c r="G43" s="6"/>
+      <c r="G43" s="4"/>
       <c r="H43" s="9">
-        <v>4.82</v>
+        <f>D43</f>
+        <v>52</v>
       </c>
       <c r="I43" s="8">
-        <f>J55/H43/24</f>
-        <v>86.445366528354086</v>
+        <f>$J$55/H43/24</f>
+        <v>8.0128205128205128</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
-      </c>
-      <c r="C44" s="5">
+        <v>36</v>
+      </c>
+      <c r="C44" s="8">
         <v>34</v>
       </c>
       <c r="D44">
         <v>52</v>
       </c>
-      <c r="E44" t="s">
-        <v>45</v>
-      </c>
-      <c r="F44" s="9">
+      <c r="E44">
+        <v>100</v>
+      </c>
+      <c r="F44" s="6">
         <f>1/5</f>
         <v>0.2</v>
       </c>
-      <c r="G44" s="4"/>
+      <c r="G44" s="4">
+        <f>(E44/1000)*F44</f>
+        <v>2.0000000000000004E-2</v>
+      </c>
       <c r="H44" s="9">
-        <f>D44</f>
-        <v>52</v>
+        <f>(G44*D44)+((1-G44)*C44)</f>
+        <v>34.36</v>
       </c>
       <c r="I44" s="8">
-        <f>J56/H44/24</f>
-        <v>8.0128205128205128</v>
+        <f t="shared" ref="I44:I48" si="2">$J$55/H44/24</f>
+        <v>12.12650368645712</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="5">
         <v>34</v>
       </c>
-      <c r="D45">
-        <v>52</v>
-      </c>
-      <c r="E45">
-        <v>100</v>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>60</v>
+      </c>
+      <c r="E45" t="s">
+        <v>59</v>
       </c>
       <c r="F45" s="6">
         <f>1/5</f>
         <v>0.2</v>
       </c>
-      <c r="G45" s="4">
-        <f t="shared" ref="G45:G49" si="2">(E45/1000)*F45</f>
-        <v>2.0000000000000004E-2</v>
-      </c>
+      <c r="G45" s="6"/>
       <c r="H45" s="9">
-        <f t="shared" ref="H45:H49" si="3">(G45*D45)+((1-G45)*C45)</f>
-        <v>34.36</v>
+        <v>4.82</v>
       </c>
       <c r="I45" s="8">
-        <f>J57/H45/24</f>
-        <v>12.12650368645712</v>
+        <f t="shared" si="2"/>
+        <v>86.445366528354086</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C46" s="5">
-        <v>4.2999999999999997E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D46">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E46">
-        <v>100</v>
-      </c>
-      <c r="F46">
-        <v>0.01</v>
+        <v>300</v>
+      </c>
+      <c r="F46" s="6">
+        <f>1/5</f>
+        <v>0.2</v>
       </c>
       <c r="G46" s="4">
+        <f>(E46/1000)*F46</f>
+        <v>0.06</v>
+      </c>
+      <c r="H46" s="9">
+        <f>(G46*D46)+((1-G46)*C46)</f>
+        <v>1.4410999999999998</v>
+      </c>
+      <c r="I46" s="8">
         <f t="shared" si="2"/>
-        <v>1E-3</v>
-      </c>
-      <c r="H46" s="9">
-        <f t="shared" si="3"/>
-        <v>5.5956999999999993E-2</v>
-      </c>
-      <c r="I46" s="8">
-        <f>J58/H46/24</f>
-        <v>7446.1938035753656</v>
+        <v>289.1309879027595</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.15">
@@ -1431,41 +1449,40 @@
         <v>0.13380500000000001</v>
       </c>
       <c r="I47" s="8">
-        <f>J59/H47/24</f>
+        <f t="shared" si="2"/>
         <v>3113.9842806073516</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C48" s="5">
-        <v>6.5000000000000002E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="D48">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="E48">
-        <v>300</v>
-      </c>
-      <c r="F48" s="6">
-        <f>1/5</f>
-        <v>0.2</v>
+        <v>100</v>
+      </c>
+      <c r="F48">
+        <v>0.01</v>
       </c>
       <c r="G48" s="4">
-        <f t="shared" ref="G48" si="4">(E48/1000)*F48</f>
-        <v>0.06</v>
+        <f>(E48/1000)*F48</f>
+        <v>1E-3</v>
       </c>
       <c r="H48" s="9">
-        <f t="shared" ref="H48" si="5">(G48*D48)+((1-G48)*C48)</f>
-        <v>1.4410999999999998</v>
+        <f>(G48*D48)+((1-G48)*C48)</f>
+        <v>5.5956999999999993E-2</v>
       </c>
       <c r="I48" s="8">
-        <f>J57/H48/24</f>
-        <v>289.1309879027595</v>
+        <f t="shared" si="2"/>
+        <v>7446.1938035753656</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.15">
@@ -1657,24 +1674,27 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E63" s="6" t="e">
+      <c r="E63" s="6">
         <f>(E44/1000)*F44</f>
-        <v>#VALUE!</v>
+        <v>2.0000000000000004E-2</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="E64" s="9" t="e">
+      <c r="E64" s="9">
         <f>1-E63</f>
-        <v>#VALUE!</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.15">
-      <c r="E65" s="6" t="e">
+      <c r="E65" s="6">
         <f>E63*D44+E64*C44</f>
-        <v>#VALUE!</v>
+        <v>34.36</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A43:I48">
+    <sortCondition ref="I43:I48"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>